<commit_message>
Working on Image Generation
This scrip will paste an image in the correct area... but it's currently
not in living colour :(
</commit_message>
<xml_diff>
--- a/Final Fantasty/DB/Ingredients.xlsx
+++ b/Final Fantasty/DB/Ingredients.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>TYPE</t>
   </si>
@@ -38,7 +38,7 @@
     <t>Spic</t>
   </si>
   <si>
-    <t>Acid</t>
+    <t>Salt</t>
   </si>
   <si>
     <t>Umami</t>
@@ -56,6 +56,12 @@
     <t>Tags</t>
   </si>
   <si>
+    <t>Card Art</t>
+  </si>
+  <si>
+    <t>Picture Location</t>
+  </si>
+  <si>
     <t>Ingredient</t>
   </si>
   <si>
@@ -68,6 +74,12 @@
     <t>tomato</t>
   </si>
   <si>
+    <t>Tomato.png</t>
+  </si>
+  <si>
+    <t>ING001</t>
+  </si>
+  <si>
     <t>Heirloom Tomato</t>
   </si>
   <si>
@@ -80,6 +92,12 @@
     <t>tomato, heirloom</t>
   </si>
   <si>
+    <t>HeirloomTomato.jpg</t>
+  </si>
+  <si>
+    <t>ING002</t>
+  </si>
+  <si>
     <t>Spaghetti</t>
   </si>
   <si>
@@ -89,6 +107,12 @@
     <t>spaghetti</t>
   </si>
   <si>
+    <t>Spaghetti.jpg</t>
+  </si>
+  <si>
+    <t>ING003</t>
+  </si>
+  <si>
     <t>Mom's Spaghetti</t>
   </si>
   <si>
@@ -96,6 +120,9 @@
   </si>
   <si>
     <t>spaghetti, moms</t>
+  </si>
+  <si>
+    <t>ING004</t>
   </si>
 </sst>
 </file>
@@ -110,6 +137,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -191,10 +219,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -210,7 +238,8 @@
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="34.6938775510204"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="24.5408163265306"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.7040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -253,16 +282,22 @@
       <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>2</v>
@@ -277,24 +312,30 @@
         <v>0</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I2" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>3</v>
@@ -308,25 +349,28 @@
       <c r="G3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="I3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="J3" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
@@ -347,21 +391,27 @@
         <v>0</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0</v>
@@ -382,7 +432,13 @@
         <v>0</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Card Generation Script v1 is complete
Still needs descriptions to be written to cards and a full slate of stat
icons but, heck we can generate cards
</commit_message>
<xml_diff>
--- a/Final Fantasty/DB/Ingredients.xlsx
+++ b/Final Fantasty/DB/Ingredients.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>TYPE</t>
   </si>
@@ -83,7 +83,7 @@
     <t>Heirloom Tomato</t>
   </si>
   <si>
-    <t>Not your mom's tomato</t>
+    <t>Not your standard tomato</t>
   </si>
   <si>
     <t>Overpowering Flavour</t>
@@ -101,6 +101,9 @@
     <t>Spaghetti</t>
   </si>
   <si>
+    <t>Pairs with thick, tomato based sauces.</t>
+  </si>
+  <si>
     <t>Al Dente</t>
   </si>
   <si>
@@ -116,7 +119,7 @@
     <t>Mom's Spaghetti</t>
   </si>
   <si>
-    <t>Just like your mother made it.</t>
+    <t>Always Ready, Mom's Spaghetti</t>
   </si>
   <si>
     <t>spaghetti, moms</t>
@@ -221,8 +224,8 @@
   </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C41" activeCellId="0" sqref="C41"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -349,6 +352,9 @@
       <c r="G3" s="0" t="n">
         <v>0</v>
       </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
       <c r="I3" s="0" t="n">
         <v>3</v>
       </c>
@@ -372,6 +378,9 @@
       <c r="B4" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="C4" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="D4" s="0" t="n">
         <v>0</v>
       </c>
@@ -391,16 +400,16 @@
         <v>0</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,10 +417,10 @@
         <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>0</v>
@@ -432,13 +441,13 @@
         <v>0</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>